<commit_message>
Update OSM features and scoping
</commit_message>
<xml_diff>
--- a/0_ref/places.xlsx
+++ b/0_ref/places.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://barnetcouncil.sharepoint.com/teams/IIHub/Shared Documents/General/02. Project Documentation/07. Standard Projects/ARC_LBB/temp/0_ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{694B1BF0-6652-4DA1-8631-48FCA7015FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94A93CE4-FC9C-4519-BA1A-696F2EBC7F85}"/>
+  <xr:revisionPtr revIDLastSave="602" documentId="8_{694B1BF0-6652-4DA1-8631-48FCA7015FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E14B1C5D-30DE-4B6E-AB92-8B199005E4EF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6D7BDA8C-7B60-475C-B43B-1BC6500B2BBC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6D7BDA8C-7B60-475C-B43B-1BC6500B2BBC}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="osm_public_transport" sheetId="3" r:id="rId4"/>
     <sheet name="osm_buildings" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">literature!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="377">
   <si>
     <t>accounting</t>
   </si>
@@ -900,9 +903,6 @@
     <t>Agricultural/Plant</t>
   </si>
   <si>
-    <t>Production</t>
-  </si>
-  <si>
     <t>barn</t>
   </si>
   <si>
@@ -1048,6 +1048,132 @@
   </si>
   <si>
     <t>buildings</t>
+  </si>
+  <si>
+    <t>Overlaps with bar and there is no biergarten in Barnet</t>
+  </si>
+  <si>
+    <t>Where there are bars, there are more people, increasing the probability of crime. Also, drinking increases the chance of accidental crime or planned crime like theft.</t>
+  </si>
+  <si>
+    <t>No place found</t>
+  </si>
+  <si>
+    <t>Same reason as bar</t>
+  </si>
+  <si>
+    <t>No evident association</t>
+  </si>
+  <si>
+    <t>Could be hotspots for vehicle crime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where there are bus stations, there are more population traffic, increasing the chance of crime. </t>
+  </si>
+  <si>
+    <t>Ther are only three places in Barnet</t>
+  </si>
+  <si>
+    <t>Ther are only two places in Barnet</t>
+  </si>
+  <si>
+    <t>Petrol station; gas station; marine fuel; … Streets to petrol stations are often tagged highway=service.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From January 2021 to February 2024, streets near or on petrol stations were hotspots for other theft in Barnet. </t>
+  </si>
+  <si>
+    <t>A container that holds grit or a mixture of salt and grit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From January 2021 to February 2024, streets near or on parking area were hotspots for violent crime in Barnet. </t>
+  </si>
+  <si>
+    <t>An entrance or exit to an underground or multi-storey parking facility. Group multiple parking entrances together with a relation using the tags type=site and site=parking. Do not mix with amenity=parking.</t>
+  </si>
+  <si>
+    <t>A single parking space. Group multiple parking spaces together with a relation using the tags type=site and site=parking. Do not mix with amenity=parking.</t>
+  </si>
+  <si>
+    <t>OSM says not to mix with parking</t>
+  </si>
+  <si>
+    <t>taxi platforms</t>
+  </si>
+  <si>
+    <t>Place where water is contained and animals can drink</t>
+  </si>
+  <si>
+    <t>Place where you can get large amounts of drinking water</t>
+  </si>
+  <si>
+    <t>Could motivate criminal behaviour</t>
+  </si>
+  <si>
+    <t>A non-bank place, where people can pay bills of public and private services and taxes.</t>
+  </si>
+  <si>
+    <t>Baby box</t>
+  </si>
+  <si>
+    <t>A facility that provides social services: group &amp; nursing homes, workshops for the disabled, homeless shelters, etc.</t>
+  </si>
+  <si>
+    <t>Discouraged tag for a home for disabled or elderly persons who need permanent care. Use amenity=social_facility + social_facility=nursing_home now.</t>
+  </si>
+  <si>
+    <t>Only 1 place found</t>
+  </si>
+  <si>
+    <t>Violent, impulsive behaviour potentially leading to crime</t>
+  </si>
+  <si>
+    <t>Only one place found</t>
+  </si>
+  <si>
+    <t>A generic public building. Don't use! See office=government.</t>
+  </si>
+  <si>
+    <t>High population traffic</t>
+  </si>
+  <si>
+    <t>From 2021 to February 2024, crimes took place most commonly on streets or near supermarket</t>
+  </si>
+  <si>
+    <t>Already captured in amenity</t>
+  </si>
+  <si>
+    <t>Overlaps with storage</t>
+  </si>
+  <si>
+    <t>A small one-room retail building.</t>
+  </si>
+  <si>
+    <t>A generic tag for a building created to house some civic amenity, for example amenity=community_centre, amenity=library, amenity=toilets, leisure=sports_centre, leisure=swimming_pool, amenity=townhall etc. Use amenity=* or leisure=* etc. to provide further details. See building=public and more specific tags like building=library as well.</t>
+  </si>
+  <si>
+    <t>A building constructed as fire station, i.e. to house fire fighting equipment and officers, regardless of current use. Add amenity=fire_station on the grounds for an active fire station.</t>
+  </si>
+  <si>
+    <t>A building constructed to be a train station building, including buildings that are abandoned and used nowadays for a different purpose.</t>
+  </si>
+  <si>
+    <t>Already captured in public transport</t>
+  </si>
+  <si>
+    <t>A building related to public transport. You will probably want to tag it with proper transport related tag as well, such as public_transport=station. Note that there is a special tag for train station buildings - building=train_station.</t>
+  </si>
+  <si>
+    <t>A garage is a building suitable for the storage of one or possibly more motor vehicle or similar. See building=garages for larger shared buildings. For an aircraft garage, see building=hangar.</t>
+  </si>
+  <si>
+    <t>A building that consists of a number of discrete storage spaces for different owners/tenants. See also building=garage.</t>
+  </si>
+  <si>
+    <t>Structure purpose-built for parking cars.</t>
+  </si>
+  <si>
+    <t>Parking space is a crime hotspot for violent crime in Barnet</t>
   </si>
 </sst>
 </file>
@@ -1094,12 +1220,14 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,6 +1244,73 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Ijgi 07 00298 g010 550">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A6851B7-3683-0194-15D7-78BFF27C7F94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3185160" y="182880"/>
+          <a:ext cx="5242560" cy="3573780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1421,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6A489B-385C-41CF-BD3B-03A2D3D989F5}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,10 +1627,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2112,7 +2307,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{3D6A489B-385C-41CF-BD3B-03A2D3D989F5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B85">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2120,17 +2321,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792D858E-8A60-490B-8B97-7151348A69CD}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="A9:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2140,7 +2344,7 @@
       </c>
       <c r="B2">
         <f>osm_amenities!C157</f>
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2154,11 +2358,19 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>335</v>
-      </c>
-      <c r="B4" s="2">
+        <v>334</v>
+      </c>
+      <c r="B4">
         <f>osm_buildings!C118</f>
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2167,7 +2379,7 @@
       </c>
       <c r="B9" s="1">
         <f>SUM(B2:B8)</f>
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2177,22 +2389,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36A0EDD-5BDC-487C-9643-376DB92603A4}">
-  <dimension ref="A1:D157"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" style="2" customWidth="1"/>
+    <col min="5" max="5" width="72.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>212</v>
       </c>
@@ -2202,1181 +2414,1868 @@
       <c r="C1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="2" t="s">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="2" t="s">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="2" t="s">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="2" t="s">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="2" t="s">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="2" t="s">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="2" t="s">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="2" t="s">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
         <v>117</v>
       </c>
-      <c r="C46" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="2" t="s">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="2" t="s">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="2" t="s">
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="2" t="s">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
         <v>121</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f>47</f>
+        <v>47</v>
+      </c>
+      <c r="B55" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>48</v>
+      </c>
+      <c r="B56" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="2" t="s">
+      <c r="E56" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>49</v>
+      </c>
+      <c r="B57" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>50</v>
+      </c>
+      <c r="B58" t="s">
         <v>125</v>
       </c>
-      <c r="C58" s="2">
-        <v>0</v>
+      <c r="C58">
+        <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
+      <c r="E58" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>51</v>
+      </c>
+      <c r="B59" t="s">
         <v>126</v>
       </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="2" t="s">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>52</v>
+      </c>
+      <c r="B60" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="2" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>53</v>
+      </c>
+      <c r="B63" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B64" s="2" t="s">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>54</v>
+      </c>
+      <c r="B64" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="2" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>55</v>
+      </c>
+      <c r="B65" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>56</v>
+      </c>
+      <c r="B66" t="s">
         <v>131</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>57</v>
+      </c>
+      <c r="B67" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="2" t="s">
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>58</v>
+      </c>
+      <c r="B68" t="s">
         <v>132</v>
       </c>
-      <c r="C68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B69" s="2" t="s">
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>59</v>
+      </c>
+      <c r="B69" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B70" s="2" t="s">
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
         <v>133</v>
       </c>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B71" s="2" t="s">
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
         <v>134</v>
       </c>
-      <c r="C71" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="2" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>62</v>
+      </c>
+      <c r="B74" t="s">
         <v>135</v>
       </c>
-      <c r="C74" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="2" t="s">
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>63</v>
+      </c>
+      <c r="B75" t="s">
         <v>136</v>
       </c>
-      <c r="C75" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B76" s="2" t="s">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>64</v>
+      </c>
+      <c r="B76" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B77" s="2" t="s">
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>65</v>
+      </c>
+      <c r="B77" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B78" s="2" t="s">
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>66</v>
+      </c>
+      <c r="B78" t="s">
         <v>139</v>
       </c>
-      <c r="C78" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B79" s="2" t="s">
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
         <v>140</v>
       </c>
-      <c r="C79" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B80" s="2" t="s">
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>68</v>
+      </c>
+      <c r="B80" t="s">
         <v>141</v>
       </c>
-      <c r="C80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="2" t="s">
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
         <v>142</v>
       </c>
-      <c r="C81" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="2" t="s">
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>70</v>
+      </c>
+      <c r="B82" t="s">
         <v>143</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82">
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="2" t="s">
+      <c r="E82" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>71</v>
+      </c>
+      <c r="B83" t="s">
         <v>144</v>
       </c>
-      <c r="C83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="2" t="s">
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>72</v>
+      </c>
+      <c r="B84" t="s">
         <v>145</v>
       </c>
-      <c r="C84" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B85" s="2" t="s">
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>73</v>
+      </c>
+      <c r="B85" t="s">
         <v>146</v>
       </c>
-      <c r="C85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B86" s="2" t="s">
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>74</v>
+      </c>
+      <c r="B86" t="s">
         <v>147</v>
       </c>
-      <c r="C86" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B87" s="2" t="s">
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>75</v>
+      </c>
+      <c r="B87" t="s">
         <v>148</v>
       </c>
-      <c r="C87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B88" s="2" t="s">
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>76</v>
+      </c>
+      <c r="B88" t="s">
         <v>149</v>
       </c>
-      <c r="C88" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="2" t="s">
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>77</v>
+      </c>
+      <c r="B89" t="s">
         <v>150</v>
       </c>
-      <c r="C89" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B90" s="2" t="s">
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>78</v>
+      </c>
+      <c r="B90" t="s">
         <v>151</v>
       </c>
-      <c r="C90" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="2" t="s">
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>79</v>
+      </c>
+      <c r="B91" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="2" t="s">
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>80</v>
+      </c>
+      <c r="B92" t="s">
         <v>153</v>
       </c>
-      <c r="C92" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B93" s="2" t="s">
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>81</v>
+      </c>
+      <c r="B93" t="s">
         <v>154</v>
       </c>
-      <c r="C93" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="2" t="s">
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>82</v>
+      </c>
+      <c r="B94" t="s">
         <v>155</v>
       </c>
-      <c r="C94" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B97" s="2" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>83</v>
+      </c>
+      <c r="B97" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B98" s="2" t="s">
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>84</v>
+      </c>
+      <c r="B98" t="s">
         <v>30</v>
       </c>
-      <c r="C98" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="2" t="s">
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>85</v>
+      </c>
+      <c r="B99" t="s">
         <v>64</v>
       </c>
-      <c r="C99" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="2" t="s">
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>86</v>
+      </c>
+      <c r="B100" t="s">
         <v>156</v>
       </c>
-      <c r="C100" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B101" s="2" t="s">
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>87</v>
+      </c>
+      <c r="B101" t="s">
         <v>157</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B102" s="2" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>88</v>
+      </c>
+      <c r="B102" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B103" s="2" t="s">
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>89</v>
+      </c>
+      <c r="B103" t="s">
         <v>158</v>
       </c>
-      <c r="C103" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B104" s="2" t="s">
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>90</v>
+      </c>
+      <c r="B104" t="s">
         <v>159</v>
       </c>
-      <c r="C104" s="2">
-        <v>1</v>
+      <c r="C104">
+        <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B105" s="2" t="s">
+      <c r="E104" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>91</v>
+      </c>
+      <c r="B105" t="s">
         <v>160</v>
       </c>
-      <c r="C105" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B108" s="2" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>92</v>
+      </c>
+      <c r="B108" t="s">
         <v>162</v>
       </c>
-      <c r="C108" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B109" s="2" t="s">
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>93</v>
+      </c>
+      <c r="B109" t="s">
         <v>163</v>
       </c>
-      <c r="C109" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B110" s="2" t="s">
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>94</v>
+      </c>
+      <c r="B110" t="s">
         <v>164</v>
       </c>
-      <c r="C110" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B111" s="2" t="s">
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>95</v>
+      </c>
+      <c r="B111" t="s">
         <v>165</v>
       </c>
-      <c r="C111" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B112" s="2" t="s">
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>96</v>
+      </c>
+      <c r="B112" t="s">
         <v>166</v>
       </c>
-      <c r="C112" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="2" t="s">
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>97</v>
+      </c>
+      <c r="B113" t="s">
         <v>167</v>
       </c>
-      <c r="C113" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="2" t="s">
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>98</v>
+      </c>
+      <c r="B114" t="s">
         <v>168</v>
       </c>
-      <c r="C114" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B115" s="2" t="s">
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>99</v>
+      </c>
+      <c r="B115" t="s">
         <v>169</v>
       </c>
-      <c r="C115" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="2" t="s">
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>100</v>
+      </c>
+      <c r="B116" t="s">
         <v>170</v>
       </c>
-      <c r="C116" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B117" s="2" t="s">
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>101</v>
+      </c>
+      <c r="B117" t="s">
         <v>171</v>
       </c>
-      <c r="C117" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="2" t="s">
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>102</v>
+      </c>
+      <c r="B118" t="s">
         <v>172</v>
       </c>
-      <c r="C118" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B119" s="2" t="s">
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>103</v>
+      </c>
+      <c r="B119" t="s">
         <v>173</v>
       </c>
-      <c r="C119" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="2" t="s">
+      <c r="C119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>104</v>
+      </c>
+      <c r="B120" t="s">
         <v>174</v>
       </c>
-      <c r="C120" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="2" t="s">
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>105</v>
+      </c>
+      <c r="B121" t="s">
         <v>175</v>
       </c>
-      <c r="C121" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="2" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
         <v>176</v>
       </c>
-      <c r="C124" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="2" t="s">
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
         <v>177</v>
       </c>
-      <c r="C125" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="2" t="s">
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
         <v>178</v>
       </c>
-      <c r="C126" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B127" s="2" t="s">
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
         <v>179</v>
       </c>
-      <c r="C127" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="2" t="s">
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
         <v>180</v>
       </c>
-      <c r="C128" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B131" s="2" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
         <v>182</v>
       </c>
-      <c r="C131" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B132" s="2" t="s">
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
         <v>183</v>
       </c>
-      <c r="C132" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B133" s="2" t="s">
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
         <v>184</v>
       </c>
-      <c r="C133" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B134" s="2" t="s">
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
         <v>185</v>
       </c>
-      <c r="C134" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B135" s="2" t="s">
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
         <v>186</v>
       </c>
-      <c r="C135" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B136" s="2" t="s">
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
         <v>187</v>
       </c>
-      <c r="C136" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B137" s="2" t="s">
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
         <v>188</v>
       </c>
-      <c r="C137" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B138" s="2" t="s">
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
         <v>189</v>
       </c>
-      <c r="C138" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B139" s="2" t="s">
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>190</v>
       </c>
-      <c r="C139" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B140" s="2" t="s">
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
         <v>191</v>
       </c>
-      <c r="C140" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B141" s="2" t="s">
+      <c r="C140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
         <v>192</v>
       </c>
-      <c r="C141" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B142" s="2" t="s">
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
         <v>193</v>
       </c>
-      <c r="C142" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B143" s="2" t="s">
+      <c r="C142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
         <v>194</v>
       </c>
-      <c r="C143" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B144" s="2" t="s">
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
         <v>195</v>
       </c>
-      <c r="C144" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B145" s="2" t="s">
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
         <v>196</v>
       </c>
-      <c r="C145" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B146" s="2" t="s">
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
         <v>197</v>
       </c>
-      <c r="C146" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B147" s="2" t="s">
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
         <v>198</v>
       </c>
-      <c r="C147" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B148" s="2" t="s">
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
         <v>199</v>
       </c>
-      <c r="C148" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B149" s="2" t="s">
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
         <v>200</v>
       </c>
-      <c r="C149" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B150" s="2" t="s">
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
         <v>201</v>
       </c>
-      <c r="C150" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B151" s="2" t="s">
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
         <v>202</v>
       </c>
-      <c r="C151" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B152" s="2" t="s">
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
         <v>203</v>
       </c>
-      <c r="C152" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B153" s="2" t="s">
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
         <v>204</v>
       </c>
-      <c r="C153" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B154" s="2" t="s">
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
         <v>205</v>
       </c>
-      <c r="C154" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B155" s="2" t="s">
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
         <v>206</v>
       </c>
-      <c r="C155" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="3" t="s">
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B157" s="3"/>
+      <c r="B157" s="4"/>
       <c r="C157" s="1">
         <f>SUM(C2:C155)</f>
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A157:B157"/>
   </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3384,10 +4283,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEB39BA-054B-4F56-A5F4-C1BD71A2C045}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3396,9 +4295,10 @@
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="93.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
@@ -3411,8 +4311,11 @@
       <c r="D1" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -3426,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>229</v>
       </c>
@@ -3439,8 +4342,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>229</v>
       </c>
@@ -3453,8 +4359,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>229</v>
       </c>
@@ -3468,12 +4377,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="1">
         <f>SUM(D2:D5)</f>
         <v>2</v>
@@ -3483,6 +4392,16 @@
   <mergeCells count="1">
     <mergeCell ref="A7:C7"/>
   </mergeCells>
+  <conditionalFormatting sqref="D1:D1048576 E1 E3:E4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3491,8 +4410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BA139E-2830-4B40-9CF6-416A338CECA1}">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3501,9 +4420,10 @@
     <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="92.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>212</v>
       </c>
@@ -3514,124 +4434,169 @@
         <v>211</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>245</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>246</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>247</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>248</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>249</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>250</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>251</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>252</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>253</v>
       </c>
       <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>254</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>255</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>256</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>257</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>258</v>
       </c>
       <c r="C16">
         <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3641,6 +4606,9 @@
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="E17" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
@@ -3649,6 +4617,9 @@
       <c r="C18">
         <v>0</v>
       </c>
+      <c r="E18" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -3657,6 +4628,9 @@
       <c r="C19">
         <v>0</v>
       </c>
+      <c r="E19" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
@@ -3665,9 +4639,12 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="E20" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3684,7 +4661,10 @@
         <v>264</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3694,6 +4674,9 @@
       <c r="C25">
         <v>1</v>
       </c>
+      <c r="D25" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -3710,10 +4693,10 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E27" s="4"/>
+      <c r="D27" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -3722,6 +4705,9 @@
       <c r="C28">
         <v>1</v>
       </c>
+      <c r="E28" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
@@ -3732,7 +4718,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3743,93 +4729,126 @@
       <c r="C32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>271</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>272</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>21</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>273</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>198</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>51</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>274</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>275</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>276</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>277</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>278</v>
       </c>
@@ -3837,47 +4856,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>279</v>
       </c>
       <c r="C46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>280</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E47" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>91</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>30</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E49" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>281</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>282</v>
       </c>
@@ -3885,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>39</v>
       </c>
@@ -3893,7 +4930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>95</v>
       </c>
@@ -3901,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>55</v>
       </c>
@@ -3909,15 +4946,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>283</v>
       </c>
       <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>70</v>
       </c>
@@ -3925,451 +4962,600 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>173</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E57" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>79</v>
       </c>
       <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>284</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>82</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>285</v>
       </c>
-      <c r="B62" t="s">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
         <v>286</v>
       </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
         <v>287</v>
       </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
         <v>288</v>
       </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
         <v>289</v>
       </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>290</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
         <v>291</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
         <v>292</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
         <v>293</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>294</v>
       </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>295</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
         <v>296</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
         <v>297</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
         <v>298</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
         <v>299</v>
       </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
-        <v>300</v>
-      </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>74</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="E79" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
+        <v>300</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
         <v>301</v>
       </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
         <v>302</v>
       </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
         <v>303</v>
       </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B85" t="s">
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
         <v>304</v>
       </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
         <v>305</v>
       </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
         <v>306</v>
       </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>307</v>
       </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
-        <v>308</v>
-      </c>
       <c r="C89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>59</v>
       </c>
       <c r="C90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>375</v>
+      </c>
+      <c r="E90" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>310</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>311</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>312</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>313</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>314</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>315</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>316</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B101" t="s">
         <v>309</v>
       </c>
-      <c r="C92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B93" t="s">
-        <v>311</v>
-      </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>312</v>
-      </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
-        <v>313</v>
-      </c>
-      <c r="C95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
-        <v>314</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
-        <v>315</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
-        <v>316</v>
-      </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
-        <v>317</v>
-      </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
         <v>318</v>
       </c>
-      <c r="B101" t="s">
-        <v>310</v>
-      </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B102" t="s">
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
         <v>319</v>
       </c>
-      <c r="C102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
         <v>320</v>
       </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="E104" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
         <v>321</v>
       </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B105" t="s">
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
         <v>322</v>
       </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B106" t="s">
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="E106" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
         <v>323</v>
       </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B107" t="s">
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="E107" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
         <v>324</v>
       </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B108" t="s">
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="E108" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
         <v>325</v>
       </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B109" t="s">
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="E109" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
         <v>326</v>
       </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B110" t="s">
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="E110" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
         <v>327</v>
       </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
         <v>328</v>
       </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B112" t="s">
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="E112" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
         <v>329</v>
       </c>
-      <c r="C112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B113" t="s">
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
         <v>330</v>
       </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B114" t="s">
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="E114" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
         <v>331</v>
       </c>
-      <c r="C114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B115" t="s">
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="E115" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
         <v>332</v>
       </c>
-      <c r="C115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B116" t="s">
-        <v>333</v>
-      </c>
       <c r="C116">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B118" s="3"/>
+      <c r="B118" s="4"/>
       <c r="C118" s="1">
         <f>SUM(C2:C116)</f>
         <v>12</v>
@@ -4379,11 +5565,41 @@
   <mergeCells count="1">
     <mergeCell ref="A118:B118"/>
   </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="47a22b0c-a034-41ca-805d-a538799fcb18" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3afbc23c-5d5f-490c-ba24-f26f24ccab85">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005DE870554D709E4B806BCA475A6F2B6F" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1db0855aec82f3c523009f75ee5aca3e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3afbc23c-5d5f-490c-ba24-f26f24ccab85" xmlns:ns3="47a22b0c-a034-41ca-805d-a538799fcb18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a8fc7a0df3c463d95ed7ba75eedf936e" ns2:_="" ns3:_="">
     <xsd:import namespace="3afbc23c-5d5f-490c-ba24-f26f24ccab85"/>
@@ -4632,36 +5848,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="47a22b0c-a034-41ca-805d-a538799fcb18" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3afbc23c-5d5f-490c-ba24-f26f24ccab85">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{016C3F1C-48D0-48B5-B1C8-E650106DBB29}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D26F8F8-1AC3-408B-9C85-5BBE92571274}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="47a22b0c-a034-41ca-805d-a538799fcb18"/>
+    <ds:schemaRef ds:uri="3afbc23c-5d5f-490c-ba24-f26f24ccab85"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C57FD711-F31C-450F-8A57-FFAE77812019}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C57FD711-F31C-450F-8A57-FFAE77812019}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D26F8F8-1AC3-408B-9C85-5BBE92571274}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{016C3F1C-48D0-48B5-B1C8-E650106DBB29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3afbc23c-5d5f-490c-ba24-f26f24ccab85"/>
+    <ds:schemaRef ds:uri="47a22b0c-a034-41ca-805d-a538799fcb18"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>